<commit_message>
Updateable household payments added
</commit_message>
<xml_diff>
--- a/public/reportTemplates/EnrollmentReportTemplate.xlsx
+++ b/public/reportTemplates/EnrollmentReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zelalemg/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zelalemg/Desktop/EHIA/CBHI/cbhi-enrollment-app/public/reportTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A211640-B4E3-AE4D-A82E-D2246BD9C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7E8921-0E0E-AE45-8BE3-336D078325CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t xml:space="preserve">  Total  </t>
   </si>
   <si>
-    <t>Copyright © 2021 Ethiopian Health Insurance Agency. All rights reserved.</t>
-  </si>
-  <si>
     <t xml:space="preserve">CBHI Scheme Enrollment Report </t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>${indigentHouseholdsWithIdCard}</t>
+  </si>
+  <si>
+    <t>Copyright © 2023-2024 Ethiopian Health Insurance Agency. All rights reserved.</t>
   </si>
 </sst>
 </file>
@@ -446,18 +446,18 @@
   <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -477,6 +477,60 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -495,7 +549,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -522,68 +576,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -611,9 +611,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -651,9 +651,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -686,26 +686,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -738,26 +721,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -933,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -945,97 +911,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="22"/>
+      <c r="A1" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="40"/>
     </row>
     <row r="2" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="22"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="40"/>
     </row>
     <row r="3" spans="1:23" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="22"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="40"/>
     </row>
     <row r="4" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
+      <c r="D4" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
       <c r="K4" s="6"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1043,32 +1009,32 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="30" t="s">
+      <c r="R4" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="V4" s="19"/>
-      <c r="W4" s="20"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" s="37"/>
+      <c r="W4" s="38"/>
     </row>
     <row r="5" spans="1:23" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
+      <c r="D5" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1084,20 +1050,20 @@
       <c r="W5" s="10"/>
     </row>
     <row r="6" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
+      <c r="D6" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1113,20 +1079,20 @@
       <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:23" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="D7" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -1142,120 +1108,120 @@
       <c r="W7" s="10"/>
     </row>
     <row r="8" spans="1:23" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="31"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
     </row>
     <row r="9" spans="1:23" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39" t="s">
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39" t="s">
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="43" t="s">
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="S9" s="44"/>
-      <c r="T9" s="41" t="s">
+      <c r="S9" s="23"/>
+      <c r="T9" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="U9" s="41" t="s">
+      <c r="U9" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="V9" s="39" t="s">
+      <c r="V9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="W9" s="39"/>
+      <c r="W9" s="20"/>
     </row>
     <row r="10" spans="1:23" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
-      <c r="B10" s="34" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="32" t="s">
+      <c r="C10" s="32"/>
+      <c r="D10" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34" t="s">
+      <c r="E10" s="27"/>
+      <c r="F10" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="32" t="s">
+      <c r="G10" s="50"/>
+      <c r="H10" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="32" t="s">
+      <c r="I10" s="27"/>
+      <c r="J10" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="32" t="s">
+      <c r="K10" s="27"/>
+      <c r="L10" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="33"/>
-      <c r="N10" s="32" t="s">
+      <c r="M10" s="27"/>
+      <c r="N10" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="33"/>
-      <c r="P10" s="32" t="s">
+      <c r="O10" s="27"/>
+      <c r="P10" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="42"/>
-      <c r="U10" s="42"/>
-      <c r="V10" s="32" t="s">
+      <c r="Q10" s="27"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="W10" s="41" t="s">
+      <c r="W10" s="21" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="9" t="s">
         <v>3</v>
       </c>
@@ -1312,83 +1278,83 @@
       </c>
       <c r="T11" s="9"/>
       <c r="U11" s="9"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="42"/>
-    </row>
-    <row r="12" spans="1:23" s="48" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V11" s="27"/>
+      <c r="W11" s="19"/>
+    </row>
+    <row r="12" spans="1:23" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="D12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="E12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="F12" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="47" t="s">
+      <c r="G12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="47" t="s">
+      <c r="H12" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="47" t="s">
+      <c r="I12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="47" t="s">
+      <c r="J12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="47" t="s">
+      <c r="K12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="47" t="s">
+      <c r="L12" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="L12" s="47" t="s">
+      <c r="M12" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="47" t="s">
+      <c r="N12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="N12" s="47" t="s">
+      <c r="O12" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="O12" s="47" t="s">
+      <c r="P12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="47" t="s">
+      <c r="Q12" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="Q12" s="47" t="s">
+      <c r="R12" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="R12" s="47" t="s">
+      <c r="S12" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="47" t="s">
+      <c r="T12" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="T12" s="49" t="s">
+      <c r="U12" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="U12" s="49" t="s">
+      <c r="V12" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="V12" s="49" t="s">
+      <c r="W12" s="17" t="s">
         <v>48</v>
-      </c>
-      <c r="W12" s="49" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="11"/>
@@ -1408,10 +1374,10 @@
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="50"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="50"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
     </row>
     <row r="14" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
@@ -1435,62 +1401,62 @@
       <c r="Q14" s="14"/>
       <c r="R14" s="14"/>
       <c r="S14" s="14"/>
-      <c r="T14" s="42"/>
-      <c r="U14" s="42"/>
-      <c r="V14" s="42"/>
-      <c r="W14" s="42"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
     </row>
     <row r="15" spans="1:23" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="17"/>
-      <c r="W15" s="18"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="35"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="36"/>
     </row>
     <row r="16" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
+      <c r="A16" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="33"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="33"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
@@ -1503,29 +1469,7 @@
       <c r="I20" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ytjp23twkUJh7467PIh8sJjeWMdJlKV8MVaahW+9i1e+CnH+sOdjBPBo42sitkBrmwfVP8tcarkJMq0wnyi6zQ==" saltValue="gikgbcEzfyt/Yguih9LouQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="37">
-    <mergeCell ref="T12:T14"/>
-    <mergeCell ref="U12:U14"/>
-    <mergeCell ref="V12:V14"/>
-    <mergeCell ref="W12:W14"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="R9:S10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
     <mergeCell ref="A16:W16"/>
     <mergeCell ref="A15:W15"/>
     <mergeCell ref="U4:W4"/>
@@ -1542,6 +1486,27 @@
     <mergeCell ref="A8:W8"/>
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="R9:S10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="T12:T14"/>
+    <mergeCell ref="U12:U14"/>
+    <mergeCell ref="V12:V14"/>
+    <mergeCell ref="W12:W14"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="W10:W11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Added enrollment excel report feature
</commit_message>
<xml_diff>
--- a/public/reportTemplates/EnrollmentReportTemplate.xlsx
+++ b/public/reportTemplates/EnrollmentReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zelalemg/Desktop/EHIA/CBHI/cbhi-enrollment-app/public/reportTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7E8921-0E0E-AE45-8BE3-336D078325CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01C2894-F1A7-8149-A758-C75D6CA545F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="90">
   <si>
     <t xml:space="preserve">Paying </t>
   </si>
@@ -69,18 +69,9 @@
     <t xml:space="preserve">Number of CBHI members newly enrolled in this  reporting period </t>
   </si>
   <si>
-    <t xml:space="preserve">Number of CBHI members newly enrolled  up to the reporting period </t>
-  </si>
-  <si>
     <t>Number of CBHI members renewed  in this reporting period</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of CBHI members renewed  upto this reporting period </t>
-  </si>
-  <si>
-    <t>Total  available members (new + renewed)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enrollment rate </t>
   </si>
   <si>
@@ -93,9 +84,6 @@
     <t xml:space="preserve">CBHI Scheme Enrollment Report </t>
   </si>
   <si>
-    <t>Number of CBHI Members</t>
-  </si>
-  <si>
     <t>Family Members (excluding HH head)</t>
   </si>
   <si>
@@ -181,6 +169,138 @@
   </si>
   <si>
     <t>Copyright © 2023-2024 Ethiopian Health Insurance Agency. All rights reserved.</t>
+  </si>
+  <si>
+    <t>Total number of CBHI members newly enrolled</t>
+  </si>
+  <si>
+    <t>Total number of CBHI members renewed</t>
+  </si>
+  <si>
+    <t>${newlyRegisteredMalePayingBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${newlyRegisteredFemalePayingBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${newlyRegisteredMaleIndigentBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${newlyRegisteredFemaleIndigentBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredMalePayingBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredFemalePayingBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredMaleIndigentBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredFemaleIndigentBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${renewedMalePayingBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${renewedFemalePayingBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${renewedMaleIndigentBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${renewedFemaleIndigentBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalRenewedMalePayingBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalRenewedFemalePayingBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalRenewedMaleIndigentBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalRenewedFemaleIndigentBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalMaleBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalFemaleBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredMalePaying}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredFemalePaying}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredMaleIndigent}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredFemaleIndigent}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredMalePayingMembers}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredFemalePayingMembers}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredMaleIndigentMembers}</t>
+  </si>
+  <si>
+    <t>${totalNewlyRegisteredFemaleIndigentMembers}</t>
+  </si>
+  <si>
+    <t>${totalRenewedMalePaying}</t>
+  </si>
+  <si>
+    <t>${totalRenewedFemalePaying}</t>
+  </si>
+  <si>
+    <t>${totalRenewedMaleIndigent}</t>
+  </si>
+  <si>
+    <t>${totalRenewedFemaleIndigent}</t>
+  </si>
+  <si>
+    <t>${totalRenewedMalePayingMembers}</t>
+  </si>
+  <si>
+    <t>${totalRenewedFemalePayingMembers}</t>
+  </si>
+  <si>
+    <t>${totalRenewedMaleIndigentMembers}</t>
+  </si>
+  <si>
+    <t>${totalRenewedFemaleIndigentMembers}</t>
+  </si>
+  <si>
+    <t>${totalMaleMembers}</t>
+  </si>
+  <si>
+    <t>${totalFemaleMembers}</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>${totalHouseholds}</t>
+  </si>
+  <si>
+    <t>${totalBeneficiaries}</t>
+  </si>
+  <si>
+    <t>${totalMembers}</t>
+  </si>
+  <si>
+    <t>Total  Active CBHI Members (New + Renewed)</t>
+  </si>
+  <si>
+    <t>Number of CBHI Members / Households</t>
   </si>
 </sst>
 </file>
@@ -190,9 +310,16 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -249,7 +376,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,8 +395,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -398,19 +531,72 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -418,6 +604,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -430,160 +640,394 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -897,111 +1341,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:X20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="23" width="8.33203125" customWidth="1"/>
-    <col min="24" max="256" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="19" width="8.33203125" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" customWidth="1"/>
+    <col min="21" max="21" width="8.33203125" customWidth="1"/>
+    <col min="22" max="22" width="10" customWidth="1"/>
+    <col min="23" max="24" width="8.33203125" customWidth="1"/>
+    <col min="25" max="257" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="40"/>
+    <row r="1" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
     </row>
-    <row r="2" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="40"/>
+    <row r="2" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="29"/>
     </row>
-    <row r="3" spans="1:23" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="40"/>
+    <row r="3" spans="1:24" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="29"/>
     </row>
-    <row r="4" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="47" t="s">
+    <row r="4" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
+      <c r="D4" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
       <c r="K4" s="6"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1009,32 +1460,33 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="48" t="s">
+      <c r="R4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="48"/>
-      <c r="T4" s="48"/>
-      <c r="U4" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="V4" s="37"/>
-      <c r="W4" s="38"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="W4" s="26"/>
+      <c r="X4" s="27"/>
     </row>
-    <row r="5" spans="1:23" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+    <row r="5" spans="1:24" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
+      <c r="D5" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1044,26 +1496,27 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
-      <c r="T5" s="4"/>
+      <c r="T5" s="2"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
-      <c r="W5" s="10"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="10"/>
     </row>
-    <row r="6" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
+    <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
+      <c r="D6" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1073,26 +1526,27 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
-      <c r="T6" s="4"/>
+      <c r="T6" s="2"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
-      <c r="W6" s="10"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="10"/>
     </row>
-    <row r="7" spans="1:23" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+    <row r="7" spans="1:24" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="46"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
+      <c r="D7" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -1105,123 +1559,127 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
-      <c r="W7" s="10"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:23" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="49"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
-      <c r="T8" s="49"/>
-      <c r="U8" s="49"/>
-      <c r="V8" s="49"/>
-      <c r="W8" s="49"/>
+    <row r="8" spans="1:24" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="62"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="38"/>
+      <c r="W8" s="38"/>
+      <c r="X8" s="38"/>
     </row>
-    <row r="9" spans="1:23" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20" t="s">
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" s="50"/>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="S9" s="64"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="V9" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20" t="s">
+      <c r="W9" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="S9" s="23"/>
-      <c r="T9" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="U9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="V9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="W9" s="20"/>
+      <c r="X9" s="41"/>
     </row>
-    <row r="10" spans="1:23" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
-      <c r="B10" s="31" t="s">
+    <row r="10" spans="1:24" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="26" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="31" t="s">
+      <c r="E10" s="16"/>
+      <c r="F10" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="50"/>
-      <c r="H10" s="26" t="s">
+      <c r="G10" s="43"/>
+      <c r="H10" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="26" t="s">
+      <c r="I10" s="45"/>
+      <c r="J10" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K10" s="27"/>
-      <c r="L10" s="26" t="s">
+      <c r="K10" s="16"/>
+      <c r="L10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="27"/>
-      <c r="N10" s="26" t="s">
+      <c r="M10" s="16"/>
+      <c r="N10" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="27"/>
-      <c r="P10" s="26" t="s">
+      <c r="O10" s="45"/>
+      <c r="P10" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="26" t="s">
+      <c r="Q10" s="61"/>
+      <c r="R10" s="66"/>
+      <c r="S10" s="67"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="59"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="W10" s="21" t="s">
+      <c r="X10" s="56" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
+    <row r="11" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
       <c r="B11" s="9" t="s">
         <v>3</v>
       </c>
@@ -1234,16 +1692,16 @@
       <c r="E11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="46" t="s">
         <v>4</v>
       </c>
       <c r="J11" s="9" t="s">
@@ -1258,205 +1716,291 @@
       <c r="M11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="N11" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="O11" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="P11" s="9" t="s">
+      <c r="P11" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="Q11" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="R11" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="S11" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="19"/>
+      <c r="T11" s="87" t="s">
+        <v>84</v>
+      </c>
+      <c r="U11" s="52"/>
+      <c r="V11" s="58"/>
+      <c r="W11" s="45"/>
+      <c r="X11" s="58"/>
     </row>
-    <row r="12" spans="1:23" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="15" t="s">
+    <row r="12" spans="1:24" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="G12" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="H12" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="I12" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="J12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="K12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="L12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="M12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="N12" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="O12" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="P12" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="Q12" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="R12" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="O12" s="15" t="s">
+      <c r="S12" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="P12" s="15" t="s">
+      <c r="T12" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="U12" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="Q12" s="15" t="s">
+      <c r="V12" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="R12" s="15" t="s">
+      <c r="W12" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="S12" s="15" t="s">
+      <c r="X12" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="T12" s="17" t="s">
+    </row>
+    <row r="13" spans="1:24" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="L13" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="M13" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="O13" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="P13" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q13" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="S13" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="T13" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="U13" s="74"/>
+      <c r="V13" s="53"/>
+      <c r="W13" s="53"/>
+      <c r="X13" s="53"/>
+    </row>
+    <row r="14" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="N14" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="O14" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="P14" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q14" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="R14" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="S14" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="T14" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="U14" s="75"/>
+      <c r="V14" s="54"/>
+      <c r="W14" s="54"/>
+      <c r="X14" s="54"/>
+    </row>
+    <row r="15" spans="1:24" ht="11" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="76"/>
+      <c r="S15" s="76"/>
+      <c r="T15" s="76"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="25"/>
+    </row>
+    <row r="16" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="U12" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="V12" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="W12" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-    </row>
-    <row r="14" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
-      <c r="V14" s="19"/>
-      <c r="W14" s="19"/>
-    </row>
-    <row r="15" spans="1:23" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="36"/>
-    </row>
-    <row r="16" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="33"/>
-      <c r="U16" s="33"/>
-      <c r="V16" s="33"/>
-      <c r="W16" s="33"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="22"/>
+      <c r="W16" s="22"/>
+      <c r="X16" s="22"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
@@ -1469,11 +2013,12 @@
       <c r="I20" s="1"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="jxMi9Tn90pVgmFiyEGc6x5IirqJTzt4bHnJppeLzNU0SC086RA+zB+7zKVpXtS3rPPJDWn+Xlb4EAp/5ydMZhA==" saltValue="3bTa82PAzCCr07vljm7p2w==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0"/>
   <mergeCells count="37">
-    <mergeCell ref="A16:W16"/>
-    <mergeCell ref="A15:W15"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="A1:W3"/>
+    <mergeCell ref="A16:X16"/>
+    <mergeCell ref="A15:X15"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="A1:X3"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="D6:J6"/>
@@ -1482,8 +2027,8 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="A8:W8"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="A8:X8"/>
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
@@ -1494,19 +2039,19 @@
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="R9:S10"/>
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="N9:Q9"/>
     <mergeCell ref="N10:O10"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="T12:T14"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="U9:U11"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="R9:T10"/>
     <mergeCell ref="U12:U14"/>
     <mergeCell ref="V12:V14"/>
     <mergeCell ref="W12:W14"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="X12:X14"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="X10:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Contribution excel report added
</commit_message>
<xml_diff>
--- a/public/reportTemplates/EnrollmentReportTemplate.xlsx
+++ b/public/reportTemplates/EnrollmentReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zelalemg/Desktop/EHIA/CBHI/cbhi-enrollment-app/public/reportTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01C2894-F1A7-8149-A758-C75D6CA545F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFFD72C-2A08-5343-844F-D783CB406875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -804,8 +804,143 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -822,103 +957,70 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -926,108 +1028,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1359,100 +1359,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="29"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="44"/>
     </row>
     <row r="2" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="29"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="44"/>
     </row>
     <row r="3" spans="1:24" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="29"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="44"/>
     </row>
     <row r="4" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="6"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1460,33 +1460,33 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="37" t="s">
+      <c r="R4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="26" t="s">
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="26"/>
-      <c r="X4" s="27"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="42"/>
     </row>
     <row r="5" spans="1:24" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="36"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1503,20 +1503,20 @@
       <c r="X5" s="10"/>
     </row>
     <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1533,20 +1533,20 @@
       <c r="X6" s="10"/>
     </row>
     <row r="7" spans="1:24" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="35"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -1563,123 +1563,123 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="62"/>
-      <c r="T8" s="62"/>
-      <c r="U8" s="38"/>
-      <c r="V8" s="38"/>
-      <c r="W8" s="38"/>
-      <c r="X8" s="38"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="53"/>
+      <c r="V8" s="53"/>
+      <c r="W8" s="53"/>
+      <c r="X8" s="53"/>
     </row>
     <row r="9" spans="1:24" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="41" t="s">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="14" t="s">
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="41" t="s">
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="O9" s="50"/>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="63" t="s">
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="S9" s="64"/>
-      <c r="T9" s="65"/>
-      <c r="U9" s="51" t="s">
+      <c r="S9" s="78"/>
+      <c r="T9" s="79"/>
+      <c r="U9" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="V9" s="56" t="s">
+      <c r="V9" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="W9" s="41" t="s">
+      <c r="W9" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="X9" s="41"/>
+      <c r="X9" s="66"/>
     </row>
     <row r="10" spans="1:24" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="63"/>
+      <c r="B10" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="15" t="s">
+      <c r="C10" s="68"/>
+      <c r="D10" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="42" t="s">
+      <c r="E10" s="61"/>
+      <c r="F10" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="44" t="s">
+      <c r="G10" s="58"/>
+      <c r="H10" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="45"/>
-      <c r="J10" s="15" t="s">
+      <c r="I10" s="59"/>
+      <c r="J10" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="15" t="s">
+      <c r="K10" s="61"/>
+      <c r="L10" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="16"/>
-      <c r="N10" s="44" t="s">
+      <c r="M10" s="61"/>
+      <c r="N10" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="45"/>
-      <c r="P10" s="44" t="s">
+      <c r="O10" s="59"/>
+      <c r="P10" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="Q10" s="61"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="68"/>
-      <c r="U10" s="59"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="44" t="s">
+      <c r="Q10" s="56"/>
+      <c r="R10" s="80"/>
+      <c r="S10" s="81"/>
+      <c r="T10" s="82"/>
+      <c r="U10" s="72"/>
+      <c r="V10" s="75"/>
+      <c r="W10" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="X10" s="56" t="s">
+      <c r="X10" s="74" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="9" t="s">
         <v>3</v>
       </c>
@@ -1692,16 +1692,16 @@
       <c r="E11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="46" t="s">
+      <c r="G11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="46" t="s">
+      <c r="I11" s="17" t="s">
         <v>4</v>
       </c>
       <c r="J11" s="9" t="s">
@@ -1716,58 +1716,58 @@
       <c r="M11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="46" t="s">
+      <c r="N11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="O11" s="46" t="s">
+      <c r="O11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="P11" s="46" t="s">
+      <c r="P11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="69" t="s">
+      <c r="Q11" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="R11" s="85" t="s">
+      <c r="R11" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="S11" s="86" t="s">
+      <c r="S11" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="T11" s="87" t="s">
+      <c r="T11" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="U11" s="52"/>
-      <c r="V11" s="58"/>
-      <c r="W11" s="45"/>
-      <c r="X11" s="58"/>
+      <c r="U11" s="73"/>
+      <c r="V11" s="76"/>
+      <c r="W11" s="59"/>
+      <c r="X11" s="76"/>
     </row>
     <row r="12" spans="1:24" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="47" t="s">
+      <c r="F12" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="48" t="s">
+      <c r="G12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="48" t="s">
+      <c r="H12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="48" t="s">
+      <c r="I12" s="19" t="s">
         <v>30</v>
       </c>
       <c r="J12" s="12" t="s">
@@ -1782,37 +1782,37 @@
       <c r="M12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="N12" s="48" t="s">
+      <c r="N12" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="O12" s="48" t="s">
+      <c r="O12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="P12" s="48" t="s">
+      <c r="P12" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Q12" s="70" t="s">
+      <c r="Q12" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="R12" s="82" t="s">
+      <c r="R12" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="S12" s="83" t="s">
+      <c r="S12" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="T12" s="84" t="s">
+      <c r="T12" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="U12" s="73" t="s">
+      <c r="U12" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="V12" s="55" t="s">
+      <c r="V12" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="W12" s="55" t="s">
+      <c r="W12" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="X12" s="55" t="s">
+      <c r="X12" s="86" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1820,67 +1820,67 @@
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="47" t="s">
+      <c r="F13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="47" t="s">
+      <c r="H13" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="47" t="s">
+      <c r="I13" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="J13" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="39" t="s">
+      <c r="K13" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="L13" s="39" t="s">
+      <c r="L13" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="M13" s="39" t="s">
+      <c r="M13" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="N13" s="47" t="s">
+      <c r="N13" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="O13" s="47" t="s">
+      <c r="O13" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="P13" s="47" t="s">
+      <c r="P13" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="Q13" s="71" t="s">
+      <c r="Q13" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="R13" s="78" t="s">
+      <c r="R13" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="S13" s="47" t="s">
+      <c r="S13" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="T13" s="77" t="s">
+      <c r="T13" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="U13" s="74"/>
-      <c r="V13" s="53"/>
-      <c r="W13" s="53"/>
-      <c r="X13" s="53"/>
+      <c r="U13" s="84"/>
+      <c r="V13" s="87"/>
+      <c r="W13" s="87"/>
+      <c r="X13" s="87"/>
     </row>
     <row r="14" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -1898,16 +1898,16 @@
       <c r="E14" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="49" t="s">
+      <c r="H14" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="49" t="s">
+      <c r="I14" s="16" t="s">
         <v>73</v>
       </c>
       <c r="J14" s="11" t="s">
@@ -1922,85 +1922,85 @@
       <c r="M14" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="N14" s="49" t="s">
+      <c r="N14" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="O14" s="49" t="s">
+      <c r="O14" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="P14" s="49" t="s">
+      <c r="P14" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="Q14" s="72" t="s">
+      <c r="Q14" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="R14" s="79" t="s">
+      <c r="R14" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="S14" s="80" t="s">
+      <c r="S14" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="T14" s="81" t="s">
+      <c r="T14" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="U14" s="75"/>
-      <c r="V14" s="54"/>
-      <c r="W14" s="54"/>
-      <c r="X14" s="54"/>
+      <c r="U14" s="85"/>
+      <c r="V14" s="88"/>
+      <c r="W14" s="88"/>
+      <c r="X14" s="88"/>
     </row>
     <row r="15" spans="1:24" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="76"/>
-      <c r="S15" s="76"/>
-      <c r="T15" s="76"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="25"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="39"/>
+      <c r="U15" s="38"/>
+      <c r="V15" s="38"/>
+      <c r="W15" s="38"/>
+      <c r="X15" s="40"/>
     </row>
     <row r="16" spans="1:24" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-      <c r="U16" s="22"/>
-      <c r="V16" s="22"/>
-      <c r="W16" s="22"/>
-      <c r="X16" s="22"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="36"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
@@ -2013,8 +2013,29 @@
       <c r="I20" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jxMi9Tn90pVgmFiyEGc6x5IirqJTzt4bHnJppeLzNU0SC086RA+zB+7zKVpXtS3rPPJDWn+Xlb4EAp/5ydMZhA==" saltValue="3bTa82PAzCCr07vljm7p2w==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="D/M3eAvtqP+6xoNPLEUlBgwVjU5RofC0GFaelgk8CH0FpytK2Ibp6ydGw2587GvVZadBeXJqsbAhWemsdlg13Q==" saltValue="1/CKHQuBVcuFWcdTV6eJag==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0"/>
   <mergeCells count="37">
+    <mergeCell ref="U12:U14"/>
+    <mergeCell ref="V12:V14"/>
+    <mergeCell ref="W12:W14"/>
+    <mergeCell ref="X12:X14"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="X10:X11"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="U9:U11"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="R9:T10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="A16:X16"/>
     <mergeCell ref="A15:X15"/>
     <mergeCell ref="V4:X4"/>
@@ -2031,27 +2052,6 @@
     <mergeCell ref="A8:X8"/>
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="U9:U11"/>
-    <mergeCell ref="V9:V11"/>
-    <mergeCell ref="R9:T10"/>
-    <mergeCell ref="U12:U14"/>
-    <mergeCell ref="V12:V14"/>
-    <mergeCell ref="W12:W14"/>
-    <mergeCell ref="X12:X14"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="X10:X11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>